<commit_message>
BOM has been updated and the items added to the mouser website
</commit_message>
<xml_diff>
--- a/Projects/Camera_System_BOM_v01.xlsx
+++ b/Projects/Camera_System_BOM_v01.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtolenti89\Documents\Projects\Kicad\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vito7253\Documents\Projects\Kicad\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="140">
   <si>
     <t>Source</t>
   </si>
@@ -426,16 +426,28 @@
     <t>Voltage</t>
   </si>
   <si>
-    <t>GRM033R61C104KE84D</t>
-  </si>
-  <si>
-    <t>0201ZD225MAT2A</t>
+    <t>06033C104K4T4A</t>
+  </si>
+  <si>
+    <t>GRM188R61C225KE15J</t>
+  </si>
+  <si>
+    <t>885012106022</t>
+  </si>
+  <si>
+    <t>VJ0603A220JXACW1BC</t>
+  </si>
+  <si>
+    <t>0805ZD226KAT2A</t>
+  </si>
+  <si>
+    <t>885012207072</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -951,7 +963,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -963,6 +975,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1320,19 +1333,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="19.85546875" customWidth="1"/>
+    <col min="2" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1348,7 +1363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1359,7 +1374,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1367,7 +1382,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1383,7 +1398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1391,7 +1406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1414,7 +1429,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1432,7 +1447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1455,7 +1470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1473,7 +1488,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1496,27 +1511,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>15</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="E15" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1528,6 +1547,9 @@
       </c>
       <c r="D16" s="2" t="s">
         <v>123</v>
+      </c>
+      <c r="E16" t="s">
+        <v>138</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -1590,7 +1612,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1608,7 +1630,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1620,6 +1642,9 @@
       </c>
       <c r="D21" s="2" t="s">
         <v>123</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="F21" t="s">
         <v>19</v>
@@ -1744,6 +1769,9 @@
       <c r="D28" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="E28" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="F28" t="s">
         <v>19</v>
       </c>
@@ -1764,6 +1792,9 @@
       <c r="D29" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="E29" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="F29" t="s">
         <v>19</v>
       </c>
@@ -1860,7 +1891,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -1896,7 +1927,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1909,6 +1940,9 @@
       <c r="D37" s="2" t="s">
         <v>123</v>
       </c>
+      <c r="E37" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="F37" t="s">
         <v>19</v>
       </c>
@@ -1916,7 +1950,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -1928,6 +1962,9 @@
       </c>
       <c r="D38" s="2" t="s">
         <v>123</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="F38" t="s">
         <v>19</v>
@@ -2004,7 +2041,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -2017,6 +2054,9 @@
       <c r="D43" s="2" t="s">
         <v>123</v>
       </c>
+      <c r="E43" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="F43" t="s">
         <v>19</v>
       </c>
@@ -2024,7 +2064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -2036,6 +2076,9 @@
       </c>
       <c r="D44" s="2" t="s">
         <v>123</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="F44" t="s">
         <v>19</v>
@@ -2079,7 +2122,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -2091,6 +2134,9 @@
       </c>
       <c r="D47" s="2" t="s">
         <v>123</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="F47" t="s">
         <v>19</v>
@@ -2134,7 +2180,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -2146,6 +2192,9 @@
       </c>
       <c r="D50" s="2" t="s">
         <v>123</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="F50" t="s">
         <v>19</v>
@@ -2382,7 +2431,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>101</v>
       </c>
@@ -2394,6 +2443,9 @@
       </c>
       <c r="D64" s="2" t="s">
         <v>123</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="F64" t="s">
         <v>19</v>
@@ -2420,7 +2472,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>104</v>
       </c>
@@ -2433,6 +2485,9 @@
       <c r="D66" s="2" t="s">
         <v>123</v>
       </c>
+      <c r="E66" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="F66" t="s">
         <v>19</v>
       </c>
@@ -2440,7 +2495,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>105</v>
       </c>
@@ -2452,6 +2507,9 @@
       </c>
       <c r="D67" s="2" t="s">
         <v>123</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="F67" t="s">
         <v>19</v>
@@ -2591,11 +2649,6 @@
         <filter val="Reference"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="0603"/>
-      </filters>
-    </filterColumn>
   </autoFilter>
   <hyperlinks>
     <hyperlink ref="E33" r:id="rId1" display="http://www.mouser.de/ProductDetail/3M-Electronic-Solutions-Division/929975-01-07/?qs=sGAEpiMZZMs%252bGHln7q6pmzaFaX6eWkWm4CFP4cdNMpU%3d"/>

</xml_diff>